<commit_message>
Aggiustati degli errori sul file name
</commit_message>
<xml_diff>
--- a/ValutazioneAnnotazioni.xlsx
+++ b/ValutazioneAnnotazioni.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiacastiello/Desktop/tesi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiacastiello/Desktop/tesi/code/PreparazioneDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{660CDD0C-996E-A74C-AE77-14AF836DE732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B6C75C-9BF6-5B48-8E97-4D45279CA137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="17060" windowHeight="9720" xr2:uid="{DF822683-9B7D-BD4E-8ECB-3A3E701B4801}"/>
+    <workbookView xWindow="17340" yWindow="940" windowWidth="17060" windowHeight="19560" xr2:uid="{DF822683-9B7D-BD4E-8ECB-3A3E701B4801}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>id annotatore</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>punteggio</t>
   </si>
   <si>
-    <t>id annotatore equivalente</t>
-  </si>
-  <si>
-    <t>19, 26</t>
+    <t>id_annotatore</t>
+  </si>
+  <si>
+    <t>id_annotatore_equivalente</t>
+  </si>
+  <si>
+    <t>20; 23</t>
+  </si>
+  <si>
+    <t>22;26</t>
+  </si>
+  <si>
+    <t>17;23</t>
+  </si>
+  <si>
+    <t>19;26</t>
+  </si>
+  <si>
+    <t>17;2</t>
+  </si>
+  <si>
+    <t>19;22</t>
   </si>
 </sst>
 </file>
@@ -422,7 +437,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,10 +447,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -600,8 +615,8 @@
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18">
-        <v>20.23</v>
+      <c r="C18" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -622,8 +637,8 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>22.26</v>
+      <c r="C20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -633,8 +648,8 @@
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21">
-        <v>17.23</v>
+      <c r="C21" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -656,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -666,8 +681,8 @@
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24">
-        <v>17.2</v>
+      <c r="C24" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -693,8 +708,8 @@
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27">
-        <v>19.22</v>
+      <c r="C27" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>